<commit_message>
DOP_19B_UAT_Segregation_of_Newly_Added_UAT's for TIV and Rasters
</commit_message>
<xml_diff>
--- a/testdata/testsheet.xlsx
+++ b/testdata/testsheet.xlsx
@@ -30,7 +30,7 @@
     <t>UHJlcHJvMQ==</t>
   </si>
   <si>
-    <t>esrrajo</t>
+    <t>automationuser</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>